<commit_message>
new version of stacker program created
</commit_message>
<xml_diff>
--- a/DoMoreReferenece.xlsx
+++ b/DoMoreReferenece.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmarshall\source\BlueMachinePLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED989926-A97F-4008-8DE4-6B24EF93C1D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E4D6D9-43CB-4B8B-8B46-E5393C1C4B89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{F6E762D9-0417-433A-93CB-4105F3298C23}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{F6E762D9-0417-433A-93CB-4105F3298C23}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="2" r:id="rId1"/>
@@ -3483,8 +3483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{604C5E72-732C-44E8-8BF0-C3EEAAC9B46D}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4238,8 +4238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AE4706-9A77-4125-8F2E-49A77C7DE771}">
   <dimension ref="B2:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>